<commit_message>
fixed integrations test refuel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -586,10 +586,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -765,7 +765,7 @@
       </c>
       <c r="E16" s="11" t="inlineStr">
         <is>
-          <t>Aktuelt</t>
+          <t>Resultat</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="E24" s="11" t="inlineStr">
         <is>
-          <t>Aktuelt</t>
+          <t>Resultat</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="E32" s="11" t="inlineStr">
         <is>
-          <t>Aktuelt</t>
+          <t>Resultat</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="E48" s="11" t="inlineStr">
         <is>
-          <t>Aktuelt</t>
+          <t>Resultat</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="E56" s="11" t="inlineStr">
         <is>
-          <t>Aktuelt</t>
+          <t>Resultat</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
     <row r="64">
       <c r="A64" s="15" t="inlineStr">
         <is>
-          <t>Test Fuel_Empty Throttle_100%</t>
+          <t>Test Refuel Throttle_100%</t>
         </is>
       </c>
       <c r="B64" s="11" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="E64" s="11" t="inlineStr">
         <is>
-          <t>Aktuelt</t>
+          <t>Resultat</t>
         </is>
       </c>
     </row>
@@ -1638,15 +1638,13 @@
           <t>currentGear</t>
         </is>
       </c>
-      <c r="B66" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="B66" s="11" t="n"/>
       <c r="C66" s="11" t="n"/>
       <c r="D66" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -1655,11 +1653,7 @@
           <t>clutchEngaged</t>
         </is>
       </c>
-      <c r="B67" s="11" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="B67" s="11" t="n"/>
       <c r="C67" s="11" t="n"/>
       <c r="D67" s="11" t="inlineStr">
         <is>
@@ -1681,18 +1675,14 @@
       <c r="B68" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="C68" s="11" t="inlineStr">
-        <is>
-          <t>0.24</t>
-        </is>
-      </c>
-      <c r="D68" s="11" t="inlineStr">
-        <is>
-          <t>0.24</t>
-        </is>
+      <c r="C68" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" s="11" t="n">
+        <v>0</v>
       </c>
       <c r="E68" s="11" t="n">
-        <v>0.24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -1706,10 +1696,10 @@
       </c>
       <c r="C69" s="11" t="n"/>
       <c r="D69" s="11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E69" s="11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70">
@@ -1718,67 +1708,20 @@
           <t>f_content</t>
         </is>
       </c>
-      <c r="B70" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C70" s="11" t="n"/>
-      <c r="D70" s="18" t="n">
-        <v>0</v>
+      <c r="B70" s="11" t="n"/>
+      <c r="C70" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D70" s="11" t="inlineStr">
+        <is>
+          <t>99.75</t>
+        </is>
       </c>
       <c r="E70" s="11" t="n">
-        <v>0</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="71"/>
-    <row r="72">
-      <c r="A72" s="15" t="n"/>
-      <c r="B72" s="11" t="n"/>
-      <c r="C72" s="11" t="n"/>
-      <c r="D72" s="11" t="n"/>
-      <c r="E72" s="11" t="n"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="13" t="n"/>
-      <c r="B73" s="11" t="n"/>
-      <c r="C73" s="11" t="n"/>
-      <c r="D73" s="11" t="n"/>
-      <c r="E73" s="11" t="n"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="13" t="n"/>
-      <c r="B74" s="11" t="n"/>
-      <c r="C74" s="11" t="n"/>
-      <c r="D74" s="11" t="n"/>
-      <c r="E74" s="11" t="n"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="13" t="n"/>
-      <c r="B75" s="11" t="n"/>
-      <c r="C75" s="11" t="n"/>
-      <c r="D75" s="11" t="n"/>
-      <c r="E75" s="11" t="n"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="13" t="n"/>
-      <c r="B76" s="11" t="n"/>
-      <c r="C76" s="11" t="n"/>
-      <c r="D76" s="11" t="n"/>
-      <c r="E76" s="11" t="n"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="13" t="n"/>
-      <c r="B77" s="11" t="n"/>
-      <c r="C77" s="11" t="n"/>
-      <c r="D77" s="11" t="n"/>
-      <c r="E77" s="11" t="n"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="13" t="n"/>
-      <c r="B78" s="11" t="n"/>
-      <c r="C78" s="11" t="n"/>
-      <c r="D78" s="18" t="n"/>
-      <c r="E78" s="11" t="n"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>